<commit_message>
Projeto bem encaminhado, sem funcionalidades novas, porém com varias questoes arrumadas
</commit_message>
<xml_diff>
--- a/Minhas_Contas.xlsx
+++ b/Minhas_Contas.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,6 +532,174 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Saida</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Churrasco</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Lazer</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>200</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>46072</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Pago</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Saida</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Facul</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Fixo</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>400</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>46072</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Pago</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Saida</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Mxrf11</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Investimento</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>90</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>46072</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Pago</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Mxrf11</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Rendimentos</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>46072</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Pago</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Entrada</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Salario</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Pagamentos</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>46072</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Pago</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Saida</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Teste</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Lazer</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>50</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>46072</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>